<commit_message>
updates in the tasks
</commit_message>
<xml_diff>
--- a/my-app/model_inference.xlsx
+++ b/my-app/model_inference.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1500,6 +1500,417 @@
         </is>
       </c>
     </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>73</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>PT271224160107</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>wwewe</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>22</v>
+      </c>
+      <c r="E40" t="inlineStr"/>
+      <c r="F40" t="inlineStr"/>
+      <c r="G40" s="2" t="n">
+        <v>45653.66744212963</v>
+      </c>
+      <c r="H40" t="n">
+        <v>0</v>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>Severe</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>74</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>PT271224161405</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>sss</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>24</v>
+      </c>
+      <c r="E41" t="inlineStr"/>
+      <c r="F41" t="inlineStr"/>
+      <c r="G41" s="2" t="n">
+        <v>45653.6764699074</v>
+      </c>
+      <c r="H41" t="n">
+        <v>0</v>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>Severe</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>75</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>PT271224161438</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>sss</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>24</v>
+      </c>
+      <c r="E42" t="inlineStr"/>
+      <c r="F42" t="inlineStr"/>
+      <c r="G42" s="2" t="n">
+        <v>45653.67685185185</v>
+      </c>
+      <c r="H42" t="n">
+        <v>0</v>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>Severe</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>76</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>PT271224162553</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>sdsad</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>23</v>
+      </c>
+      <c r="E43" t="inlineStr"/>
+      <c r="F43" t="inlineStr"/>
+      <c r="G43" s="2" t="n">
+        <v>45653.6846412037</v>
+      </c>
+      <c r="H43" t="n">
+        <v>0</v>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>Severe</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>77</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>PT271224162714</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>qqqwee</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>12</v>
+      </c>
+      <c r="E44" t="inlineStr"/>
+      <c r="F44" t="inlineStr"/>
+      <c r="G44" s="2" t="n">
+        <v>45653.68557870371</v>
+      </c>
+      <c r="H44" t="n">
+        <v>0</v>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>Severe</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>78</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>PT271224171633</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>www</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>23</v>
+      </c>
+      <c r="E45" t="inlineStr"/>
+      <c r="F45" t="inlineStr"/>
+      <c r="G45" s="2" t="n">
+        <v>45653.71982638889</v>
+      </c>
+      <c r="H45" t="n">
+        <v>0</v>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>Severe</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>79</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>PT271224171848</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>qeqqdsdd</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>33</v>
+      </c>
+      <c r="E46" t="inlineStr"/>
+      <c r="F46" t="inlineStr"/>
+      <c r="G46" s="2" t="n">
+        <v>45653.7216550926</v>
+      </c>
+      <c r="H46" t="n">
+        <v>2</v>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>Severe</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>82</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>PT271224172242</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>qqq</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>33</v>
+      </c>
+      <c r="E47" t="inlineStr"/>
+      <c r="F47" t="inlineStr"/>
+      <c r="G47" s="2" t="n">
+        <v>45653.72439814815</v>
+      </c>
+      <c r="H47" t="n">
+        <v>5</v>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>Severe</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>85</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>PT271224174848</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>wer</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>23</v>
+      </c>
+      <c r="E48" t="inlineStr"/>
+      <c r="F48" t="inlineStr"/>
+      <c r="G48" s="2" t="n">
+        <v>45653.74231481482</v>
+      </c>
+      <c r="H48" t="n">
+        <v>0</v>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>Severe</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>87</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>PT271224174028</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>ff</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>12</v>
+      </c>
+      <c r="E49" t="inlineStr"/>
+      <c r="F49" t="inlineStr"/>
+      <c r="G49" s="2" t="n">
+        <v>45653.74271990741</v>
+      </c>
+      <c r="H49" t="n">
+        <v>3</v>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>Severe</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>88</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>PT271224175343</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>ffff</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>22</v>
+      </c>
+      <c r="E50" t="inlineStr"/>
+      <c r="F50" t="inlineStr"/>
+      <c r="G50" s="2" t="n">
+        <v>45653.74563657407</v>
+      </c>
+      <c r="H50" t="n">
+        <v>0</v>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>Severe</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>89</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>PT271224180528</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>DGP</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>25</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>dementia</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="G51" s="2" t="n">
+        <v>45653.75569444444</v>
+      </c>
+      <c r="H51" t="n">
+        <v>28</v>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>May be Normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>92</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>PT271224181048</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>sos</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>88</v>
+      </c>
+      <c r="E52" t="inlineStr"/>
+      <c r="F52" t="inlineStr"/>
+      <c r="G52" s="2" t="n">
+        <v>45653.7575</v>
+      </c>
+      <c r="H52" t="n">
+        <v>0</v>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>Severe</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
updates to the final
</commit_message>
<xml_diff>
--- a/my-app/model_inference.xlsx
+++ b/my-app/model_inference.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I57"/>
+  <dimension ref="A1:I66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2066,6 +2066,301 @@
         </is>
       </c>
     </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>98</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>PT301224163607</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>dfdgg</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>34</v>
+      </c>
+      <c r="E58" t="inlineStr"/>
+      <c r="F58" t="inlineStr"/>
+      <c r="G58" s="2" t="n">
+        <v>45656.69174768519</v>
+      </c>
+      <c r="H58" t="n">
+        <v>0</v>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>Severe</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>99</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>PT301224163630</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>gg</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>55</v>
+      </c>
+      <c r="E59" t="inlineStr"/>
+      <c r="F59" t="inlineStr"/>
+      <c r="G59" s="2" t="n">
+        <v>45656.69201388889</v>
+      </c>
+      <c r="H59" t="n">
+        <v>0</v>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>Severe</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>100</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>PT301224163705</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>qq</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>1</v>
+      </c>
+      <c r="E60" t="inlineStr"/>
+      <c r="F60" t="inlineStr"/>
+      <c r="G60" s="2" t="n">
+        <v>45656.69241898148</v>
+      </c>
+      <c r="H60" t="n">
+        <v>0</v>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>Severe</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>101</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>PT301224163741</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>ww</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>2</v>
+      </c>
+      <c r="E61" t="inlineStr"/>
+      <c r="F61" t="inlineStr"/>
+      <c r="G61" s="2" t="n">
+        <v>45656.69283564815</v>
+      </c>
+      <c r="H61" t="n">
+        <v>0</v>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>Severe</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>102</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>PT301224164034</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>1</v>
+      </c>
+      <c r="E62" t="inlineStr"/>
+      <c r="F62" t="inlineStr"/>
+      <c r="G62" s="2" t="n">
+        <v>45656.69483796296</v>
+      </c>
+      <c r="H62" t="n">
+        <v>0</v>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>Severe</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>103</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>PT301224165257</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>qa</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>23</v>
+      </c>
+      <c r="E63" t="inlineStr"/>
+      <c r="F63" t="inlineStr"/>
+      <c r="G63" s="2" t="n">
+        <v>45656.7034375</v>
+      </c>
+      <c r="H63" t="n">
+        <v>0</v>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>Severe</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>104</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>PT301224165412</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>qq</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>22</v>
+      </c>
+      <c r="E64" t="inlineStr"/>
+      <c r="F64" t="inlineStr"/>
+      <c r="G64" s="2" t="n">
+        <v>45656.70430555556</v>
+      </c>
+      <c r="H64" t="n">
+        <v>0</v>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>Severe</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>105</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>PT301224165530</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>az</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>45</v>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>mci</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="G65" s="2" t="n">
+        <v>45656.70572916666</v>
+      </c>
+      <c r="H65" t="n">
+        <v>0</v>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>Severe</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>108</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>PT301224170458</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>rt</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>6</v>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>mci</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>Dementia</t>
+        </is>
+      </c>
+      <c r="G66" s="2" t="n">
+        <v>45656.71229166666</v>
+      </c>
+      <c r="H66" t="n">
+        <v>0</v>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>Severe</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
updates to the final; error checking
</commit_message>
<xml_diff>
--- a/my-app/model_inference.xlsx
+++ b/my-app/model_inference.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I66"/>
+  <dimension ref="A1:I70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2361,6 +2361,138 @@
         </is>
       </c>
     </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>111</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>PT301224170951</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>debolina</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>25</v>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>mci</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="G67" s="2" t="n">
+        <v>45656.71918981482</v>
+      </c>
+      <c r="H67" t="n">
+        <v>29</v>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>May be Normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>114</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>PT301224171900</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>4</v>
+      </c>
+      <c r="E68" t="inlineStr"/>
+      <c r="F68" t="inlineStr"/>
+      <c r="G68" s="2" t="n">
+        <v>45656.72152777778</v>
+      </c>
+      <c r="H68" t="n">
+        <v>0</v>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>Severe</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>115</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>PT301224171947</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>5</v>
+      </c>
+      <c r="E69" t="inlineStr"/>
+      <c r="F69" t="inlineStr"/>
+      <c r="G69" s="2" t="n">
+        <v>45656.72207175926</v>
+      </c>
+      <c r="H69" t="n">
+        <v>0</v>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>Severe</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>116</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>PT301224172258</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>2</v>
+      </c>
+      <c r="E70" t="inlineStr"/>
+      <c r="F70" t="inlineStr"/>
+      <c r="G70" s="2" t="n">
+        <v>45656.72428240741</v>
+      </c>
+      <c r="H70" t="n">
+        <v>0</v>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>Severe</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>